<commit_message>
DATA MAPPING ADDITION - PACKETBEAT
</commit_message>
<xml_diff>
--- a/machine-learning/ML-DATA/LOG-DATA-DICTIONARY.xlsx
+++ b/machine-learning/ML-DATA/LOG-DATA-DICTIONARY.xlsx
@@ -5,19 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mbpro/Desktop/PORTFOLIO/AIOps/ML-DATA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mbpro/Desktop/ELK/AIOps/machine-learning/ML-DATA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E33300-0955-0149-B9BB-52F01E9BBE59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5435A5-9F91-3C4B-9EBD-5A7DB56F1060}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="2060" windowWidth="27640" windowHeight="16940" activeTab="2" xr2:uid="{DDDE1EC0-9918-6045-A554-B75C000F315D}"/>
+    <workbookView xWindow="3180" yWindow="2060" windowWidth="27640" windowHeight="16940" activeTab="3" xr2:uid="{DDDE1EC0-9918-6045-A554-B75C000F315D}"/>
   </bookViews>
   <sheets>
     <sheet name="syslog" sheetId="1" r:id="rId1"/>
     <sheet name="dockerlog" sheetId="2" r:id="rId2"/>
     <sheet name="dockermetrics" sheetId="3" r:id="rId3"/>
+    <sheet name="packetbeats" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="511">
   <si>
     <t>@timestamp</t>
   </si>
@@ -1248,13 +1249,331 @@
   </si>
   <si>
     <t>user.name</t>
+  </si>
+  <si>
+    <t>client.bytes</t>
+  </si>
+  <si>
+    <t>client.ip</t>
+  </si>
+  <si>
+    <t>client.port</t>
+  </si>
+  <si>
+    <t>destination.bytes</t>
+  </si>
+  <si>
+    <t>destination.domain</t>
+  </si>
+  <si>
+    <t>destination.ip</t>
+  </si>
+  <si>
+    <t>destination.packets</t>
+  </si>
+  <si>
+    <t>destination.port</t>
+  </si>
+  <si>
+    <t>dns.additionals_count</t>
+  </si>
+  <si>
+    <t>dns.answers_count</t>
+  </si>
+  <si>
+    <t>dns.authorities_count</t>
+  </si>
+  <si>
+    <t>dns.flags.authentic_data</t>
+  </si>
+  <si>
+    <t>dns.flags.authoritative</t>
+  </si>
+  <si>
+    <t>dns.flags.checking_disabled</t>
+  </si>
+  <si>
+    <t>dns.flags.recursion_available</t>
+  </si>
+  <si>
+    <t>dns.flags.recursion_desired</t>
+  </si>
+  <si>
+    <t>dns.flags.truncated_response</t>
+  </si>
+  <si>
+    <t>dns.header_flags</t>
+  </si>
+  <si>
+    <t>dns.id</t>
+  </si>
+  <si>
+    <t>dns.op_code</t>
+  </si>
+  <si>
+    <t>dns.question.class</t>
+  </si>
+  <si>
+    <t>dns.question.etld_plus_one</t>
+  </si>
+  <si>
+    <t>dns.question.name</t>
+  </si>
+  <si>
+    <t>dns.question.registered_domain</t>
+  </si>
+  <si>
+    <t>dns.question.type</t>
+  </si>
+  <si>
+    <t>dns.resolved_ip</t>
+  </si>
+  <si>
+    <t>dns.response_code</t>
+  </si>
+  <si>
+    <t>dns.type</t>
+  </si>
+  <si>
+    <t>event.action</t>
+  </si>
+  <si>
+    <t>event.category</t>
+  </si>
+  <si>
+    <t>event.end</t>
+  </si>
+  <si>
+    <t>event.kind</t>
+  </si>
+  <si>
+    <t>event.start</t>
+  </si>
+  <si>
+    <t>flow.final</t>
+  </si>
+  <si>
+    <t>flow.id</t>
+  </si>
+  <si>
+    <t>http.request.body.bytes</t>
+  </si>
+  <si>
+    <t>http.request.bytes</t>
+  </si>
+  <si>
+    <t>http.request.headers.accept</t>
+  </si>
+  <si>
+    <t>http.request.headers.accept-encoding</t>
+  </si>
+  <si>
+    <t>http.request.headers.accept-language</t>
+  </si>
+  <si>
+    <t>http.request.headers.authorization</t>
+  </si>
+  <si>
+    <t>http.request.headers.connection</t>
+  </si>
+  <si>
+    <t>http.request.headers.content-length</t>
+  </si>
+  <si>
+    <t>http.request.headers.content-type</t>
+  </si>
+  <si>
+    <t>http.request.headers.host</t>
+  </si>
+  <si>
+    <t>http.request.headers.if-none-match</t>
+  </si>
+  <si>
+    <t>http.request.headers.kbn-version</t>
+  </si>
+  <si>
+    <t>http.request.headers.origin</t>
+  </si>
+  <si>
+    <t>http.request.headers.referer</t>
+  </si>
+  <si>
+    <t>http.request.headers.user-agent</t>
+  </si>
+  <si>
+    <t>http.request.method</t>
+  </si>
+  <si>
+    <t>http.request.referrer</t>
+  </si>
+  <si>
+    <t>http.response.body.bytes</t>
+  </si>
+  <si>
+    <t>http.response.bytes</t>
+  </si>
+  <si>
+    <t>http.response.headers.accept-ranges</t>
+  </si>
+  <si>
+    <t>http.response.headers.cache-control</t>
+  </si>
+  <si>
+    <t>http.response.headers.connection</t>
+  </si>
+  <si>
+    <t>http.response.headers.content-encoding</t>
+  </si>
+  <si>
+    <t>http.response.headers.content-length</t>
+  </si>
+  <si>
+    <t>http.response.headers.content-security-policy</t>
+  </si>
+  <si>
+    <t>http.response.headers.content-type</t>
+  </si>
+  <si>
+    <t>http.response.headers.date</t>
+  </si>
+  <si>
+    <t>http.response.headers.etag</t>
+  </si>
+  <si>
+    <t>http.response.headers.kbn-name</t>
+  </si>
+  <si>
+    <t>http.response.headers.kbn-xpack-sig</t>
+  </si>
+  <si>
+    <t>http.response.headers.location</t>
+  </si>
+  <si>
+    <t>http.response.headers.transfer-encoding</t>
+  </si>
+  <si>
+    <t>http.response.headers.vary</t>
+  </si>
+  <si>
+    <t>http.response.status_code</t>
+  </si>
+  <si>
+    <t>http.response.status_phrase</t>
+  </si>
+  <si>
+    <t>http.version</t>
+  </si>
+  <si>
+    <t>icmp.request.code</t>
+  </si>
+  <si>
+    <t>icmp.request.message</t>
+  </si>
+  <si>
+    <t>icmp.request.type</t>
+  </si>
+  <si>
+    <t>icmp.response.code</t>
+  </si>
+  <si>
+    <t>icmp.response.message</t>
+  </si>
+  <si>
+    <t>icmp.response.type</t>
+  </si>
+  <si>
+    <t>icmp.version</t>
+  </si>
+  <si>
+    <t>method</t>
+  </si>
+  <si>
+    <t>network.bytes</t>
+  </si>
+  <si>
+    <t>network.community_id</t>
+  </si>
+  <si>
+    <t>network.direction</t>
+  </si>
+  <si>
+    <t>network.packets</t>
+  </si>
+  <si>
+    <t>network.protocol</t>
+  </si>
+  <si>
+    <t>network.transport</t>
+  </si>
+  <si>
+    <t>network.type</t>
+  </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
+    <t>query</t>
+  </si>
+  <si>
+    <t>resource</t>
+  </si>
+  <si>
+    <t>server.bytes</t>
+  </si>
+  <si>
+    <t>server.domain</t>
+  </si>
+  <si>
+    <t>server.ip</t>
+  </si>
+  <si>
+    <t>server.port</t>
+  </si>
+  <si>
+    <t>source.bytes</t>
+  </si>
+  <si>
+    <t>source.ip</t>
+  </si>
+  <si>
+    <t>source.packets</t>
+  </si>
+  <si>
+    <t>source.port</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>url.domain</t>
+  </si>
+  <si>
+    <t>url.full</t>
+  </si>
+  <si>
+    <t>url.path</t>
+  </si>
+  <si>
+    <t>url.port</t>
+  </si>
+  <si>
+    <t>url.query</t>
+  </si>
+  <si>
+    <t>url.scheme</t>
+  </si>
+  <si>
+    <t>user_agent.original</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1266,6 +1585,13 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1291,9 +1617,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2381,8 +2708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78601CBF-85EE-D648-912A-802893F5C2E9}">
   <dimension ref="A1:D343"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4117,4 +4444,644 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9353C15-E626-5841-AB62-8E35C28C684A}">
+  <dimension ref="A1:D122"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="39.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="3" max="3" width="36" customWidth="1"/>
+    <col min="4" max="4" width="25.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" s="2" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" s="2" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" s="2" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" s="2" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" s="2" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" s="2" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" s="2" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" s="2" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" s="2" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" s="2" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" s="2" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" s="2" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" s="2" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" s="2" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" s="2" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" s="2" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74" s="2" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75" s="2" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76" s="2" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78" s="2" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" s="2" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A80" s="2" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81" s="2" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82" s="2" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83" s="2" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A84" s="2" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A85" s="2" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A86" s="2" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A87" s="2" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A88" s="2" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A89" s="2" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A90" s="2" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A91" s="2" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A92" s="2" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A93" s="2" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A94" s="2" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A95" s="2" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A96" s="2" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A97" s="2" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A98" s="2" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A99" s="2" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A100" s="2" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A101" s="2" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A102" s="2" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A103" s="2" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A104" s="2" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A105" s="2" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A106" s="2" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A107" s="2" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A108" s="2" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A109" s="2" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A110" s="2" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A111" s="2" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A112" s="2" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A113" s="2" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A114" s="2" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A115" s="2" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A116" s="2" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A117" s="2" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A118" s="2" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A119" s="2" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A120" s="2" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A121" s="2" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A122" s="2" t="s">
+        <v>510</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>